<commit_message>
Update DDS401 Team NI Case Study 1 Project Plan.xlsx
</commit_message>
<xml_diff>
--- a/DDS401 Team NI Case Study 1 Project Plan.xlsx
+++ b/DDS401 Team NI Case Study 1 Project Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa384dc48f87cf2c/Desktop/SMU MSDS/Doing Data Science/Case Study 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ruben\Documents\SMU\Ruben-Chavez-SMU-Homework\Ruben-Chavez-SMU-MSDS-Homework\Doing Data Science\DDS_401_TeamNI_Case_Study1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEC0EE55-DA5C-44A9-B24A-5106B2F4BC77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB88C2A-2C0D-44F1-B979-4F01F8C0CE1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{F80FE941-AA38-415F-98DF-929EB2B73926}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{F80FE941-AA38-415F-98DF-929EB2B73926}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Turn in and present project</t>
+  </si>
+  <si>
+    <t>Ruben Chavez</t>
   </si>
 </sst>
 </file>
@@ -607,18 +610,18 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -652,7 +655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -666,7 +669,7 @@
         <v>43453</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -677,13 +680,16 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
       <c r="D5" s="2">
         <v>43471</v>
       </c>
@@ -691,13 +697,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" s="2">
         <v>43471</v>
       </c>
@@ -705,13 +714,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
       <c r="D7" s="2">
         <v>43471</v>
       </c>
@@ -719,13 +731,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="2">
         <v>43471</v>
       </c>
@@ -733,13 +748,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="2">
         <v>43471</v>
       </c>
@@ -747,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -761,7 +779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -775,7 +793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -789,7 +807,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -800,7 +818,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -814,7 +832,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>

</xml_diff>